<commit_message>
fixed consistency, made objective smaller. and made the rigidbody on player instead of all the objectives also added the reset for all gameObjects for the maze and instantiate the in a seperate function instead of repeating the same code
</commit_message>
<xml_diff>
--- a/Hour log/DTT-Assessment-Hour-Log.xlsx
+++ b/Hour log/DTT-Assessment-Hour-Log.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tool\Downloads\DTT Assessment - Unity - 2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Repositories\MazeGenerator\Hour log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3249112-EF2E-4F71-937C-4ED6258C0E80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B713E577-8BF5-4B67-8CB8-2B21124D3B7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DTT Test Hour Log" sheetId="1" r:id="rId1"/>
@@ -26,15 +26,12 @@
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Subject</t>
   </si>
@@ -107,6 +104,27 @@
   </si>
   <si>
     <t>changed the button size to fit all</t>
+  </si>
+  <si>
+    <t>Making Inputfields</t>
+  </si>
+  <si>
+    <t>making input fields for height and width of the maze that change when you regenerate the maze. Also fixing the cameracontrols to always change based on the settings. Also setting a default so that it always shows a maze when pressing generate</t>
+  </si>
+  <si>
+    <t>Making MazeGame a game</t>
+  </si>
+  <si>
+    <t>Getting a player and an objective in</t>
+  </si>
+  <si>
+    <t>Resetting player and objectives</t>
+  </si>
+  <si>
+    <t>Making sure the players and objectives are reset once you press generate. Also fixed some small issues with objective and player collision</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -1723,8 +1741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1778,7 +1796,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" s="17">
         <v>45072</v>
@@ -1821,7 +1839,7 @@
       <c r="E6" s="19"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:6" ht="27" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
@@ -1839,7 +1857,7 @@
       </c>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>16</v>
       </c>
@@ -1855,31 +1873,59 @@
       <c r="E8" s="19"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="21"/>
+    <row r="9" spans="1:6" ht="45.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="16">
+        <v>2</v>
+      </c>
+      <c r="C9" s="17">
+        <v>45076</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>19</v>
+      </c>
       <c r="E9" s="19"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="19"/>
+    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="16">
+        <v>3</v>
+      </c>
+      <c r="C10" s="17">
+        <v>45076</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>15</v>
+      </c>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="19"/>
+    <row r="11" spans="1:6" ht="39.75" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="16">
+        <v>1</v>
+      </c>
+      <c r="C11" s="17">
+        <v>45079</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>24</v>
+      </c>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5"/>
       <c r="B12" s="16"/>
       <c r="C12" s="17"/>
@@ -2029,7 +2075,7 @@
       </c>
       <c r="B30" s="14">
         <f>SUMIF(E4:E28,"&lt;&gt;x",B4:B28)</f>
-        <v>4.2</v>
+        <v>7.2</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>

</xml_diff>

<commit_message>
changed default to 30/30 and added limiters to creation
</commit_message>
<xml_diff>
--- a/Hour log/DTT-Assessment-Hour-Log.xlsx
+++ b/Hour log/DTT-Assessment-Hour-Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Repositories\MazeGenerator\Hour log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B699C8B-8249-4B72-9A0B-F643A23B7E5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA156FBF-B28C-4F75-B839-1EF26396FB2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>Subject</t>
   </si>
@@ -125,6 +125,24 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>Added limiters to the fields</t>
+  </si>
+  <si>
+    <t>Attempting to generate second Maze</t>
+  </si>
+  <si>
+    <t>Attempting to made the player able to go trough the wall if they're the same color</t>
+  </si>
+  <si>
+    <t>Tried adding kruskal's algoritm to generate the maze, ended up running into too many issues to fix within scope</t>
+  </si>
+  <si>
+    <t>Attempted to fix the Color Maze game to have a unique mechanic of having the player go trough the wall but ended up having too many issues with movement. The objects can assign colors</t>
+  </si>
+  <si>
+    <t>Made it so there is a minimum and a maximum to maze size. Also made them changeable in the unity editor</t>
   </si>
 </sst>
 </file>
@@ -1741,8 +1759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1791,7 +1809,7 @@
       </c>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:6" ht="56.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="63.75" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>7</v>
       </c>
@@ -1807,7 +1825,7 @@
       <c r="E4" s="19"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:6" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="39.75" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
@@ -1823,7 +1841,7 @@
       <c r="E5" s="19"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:6" ht="57" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="78" x14ac:dyDescent="0.35">
       <c r="A6" s="18" t="s">
         <v>11</v>
       </c>
@@ -1839,7 +1857,7 @@
       <c r="E6" s="19"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="27" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
@@ -1857,7 +1875,7 @@
       </c>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>16</v>
       </c>
@@ -1873,7 +1891,7 @@
       <c r="E8" s="19"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:6" ht="45.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="52.5" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>18</v>
       </c>
@@ -1889,7 +1907,7 @@
       <c r="E9" s="19"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>20</v>
       </c>
@@ -1907,7 +1925,7 @@
       </c>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="39.75" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>22</v>
       </c>
@@ -1925,27 +1943,55 @@
       </c>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="19"/>
+    <row r="12" spans="1:6" ht="27" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="16">
+        <v>3</v>
+      </c>
+      <c r="C12" s="17">
+        <v>45079</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>24</v>
+      </c>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="19"/>
+    <row r="13" spans="1:6" ht="39.75" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="16">
+        <v>2</v>
+      </c>
+      <c r="C13" s="17">
+        <v>45079</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>24</v>
+      </c>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="21"/>
+    <row r="14" spans="1:6" ht="27" x14ac:dyDescent="0.35">
+      <c r="A14" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="16">
+        <v>2</v>
+      </c>
+      <c r="C14" s="17">
+        <v>45079</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>30</v>
+      </c>
       <c r="E14" s="19"/>
       <c r="F14" s="4"/>
     </row>
@@ -2075,7 +2121,7 @@
       </c>
       <c r="B30" s="14">
         <f>SUMIF(E4:E28,"&lt;&gt;x",B4:B28)</f>
-        <v>7.2</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>

</xml_diff>